<commit_message>
update with UI duration data
</commit_message>
<xml_diff>
--- a/ct_energy_events_by_zipcode.xlsx
+++ b/ct_energy_events_by_zipcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssmg/Documents/mit-policy-hack-2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43C9BE4-1B4E-4B42-B1CD-E36C0784415F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895C1CEE-0D19-934A-9043-0632A8C2E301}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="3220" windowWidth="20480" windowHeight="16940" xr2:uid="{88F03919-88F7-6043-9A91-A7D2CA2CD04D}"/>
+    <workbookView xWindow="20160" yWindow="1800" windowWidth="20480" windowHeight="16940" xr2:uid="{88F03919-88F7-6043-9A91-A7D2CA2CD04D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="521">
   <si>
     <t>TOWN</t>
   </si>
@@ -1572,9 +1572,6 @@
     <t>ZIPCODES</t>
   </si>
   <si>
-    <t>06824,06825,06828</t>
-  </si>
-  <si>
     <t>06484</t>
   </si>
   <si>
@@ -1585,6 +1582,12 @@
   </si>
   <si>
     <t>AboveAverage</t>
+  </si>
+  <si>
+    <t>06825</t>
+  </si>
+  <si>
+    <t>06828</t>
   </si>
 </sst>
 </file>
@@ -1687,7 +1690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1723,6 +1726,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2038,11 +2047,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA410DFE-5E10-0944-A5A1-460B3BB91D5E}">
-  <dimension ref="A1:K276"/>
+  <dimension ref="A1:K278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I267" sqref="I267:I272"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11319,7 +11328,7 @@
         <v>13700</v>
       </c>
       <c r="H258" s="7">
-        <f t="shared" ref="H258:H272" si="12">E258/G258</f>
+        <f t="shared" ref="H258:H274" si="12">E258/G258</f>
         <v>3.2846715328467155E-2</v>
       </c>
       <c r="I258" s="2" t="str">
@@ -11327,7 +11336,7 @@
         <v>BelowAverage</v>
       </c>
       <c r="J258" s="2" t="str">
-        <f t="shared" ref="J258:J265" si="14">IF(D258&gt;$B$3,"Above Average","BelowAverage")</f>
+        <f t="shared" ref="J258:J267" si="14">IF(D258&gt;$B$3,"Above Average","BelowAverage")</f>
         <v>BelowAverage</v>
       </c>
       <c r="K258" t="s">
@@ -11593,6 +11602,12 @@
       <c r="B266" s="13" t="s">
         <v>507</v>
       </c>
+      <c r="C266" s="18">
+        <v>242.67</v>
+      </c>
+      <c r="D266" s="17">
+        <v>710787</v>
+      </c>
       <c r="E266" s="10">
         <v>497</v>
       </c>
@@ -11607,9 +11622,12 @@
         <v>0.16968248548992831</v>
       </c>
       <c r="I266" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="J266" s="16"/>
+        <v>518</v>
+      </c>
+      <c r="J266" s="16" t="str">
+        <f t="shared" si="14"/>
+        <v>BelowAverage</v>
+      </c>
       <c r="K266" t="s">
         <v>513</v>
       </c>
@@ -11621,6 +11639,12 @@
       <c r="B267" s="13" t="s">
         <v>497</v>
       </c>
+      <c r="C267" s="18">
+        <v>158.09</v>
+      </c>
+      <c r="D267" s="17">
+        <v>589047</v>
+      </c>
       <c r="E267" s="10">
         <v>621</v>
       </c>
@@ -11635,9 +11659,12 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="I267" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="J267" s="16"/>
+        <v>518</v>
+      </c>
+      <c r="J267" s="16" t="str">
+        <f>IF(D268&gt;$B$3,"Above Average","BelowAverage")</f>
+        <v>BelowAverage</v>
+      </c>
       <c r="K267" t="s">
         <v>513</v>
       </c>
@@ -11647,7 +11674,13 @@
         <v>135</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>515</v>
+        <v>136</v>
+      </c>
+      <c r="C268" s="18">
+        <v>161.97</v>
+      </c>
+      <c r="D268" s="17">
+        <v>3643312</v>
       </c>
       <c r="E268" s="10">
         <v>1293</v>
@@ -11659,11 +11692,11 @@
         <v>22494</v>
       </c>
       <c r="H268" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="H268" si="15">E268/G268</f>
         <v>5.748199519871966E-2</v>
       </c>
       <c r="I268" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J268" s="16"/>
       <c r="K268" t="s">
@@ -11672,26 +11705,32 @@
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" s="9" t="s">
-        <v>510</v>
+        <v>135</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>516</v>
+        <v>519</v>
+      </c>
+      <c r="C269" s="18">
+        <v>161.97</v>
+      </c>
+      <c r="D269" s="17">
+        <v>3643312</v>
       </c>
       <c r="E269" s="10">
-        <v>708</v>
-      </c>
-      <c r="F269" s="14">
-        <v>84933</v>
+        <v>1293</v>
+      </c>
+      <c r="F269">
+        <v>137560</v>
       </c>
       <c r="G269" s="11">
-        <v>18709</v>
+        <v>22494</v>
       </c>
       <c r="H269" s="12">
-        <f t="shared" si="12"/>
-        <v>3.7842749478860439E-2</v>
+        <f t="shared" ref="H269" si="16">E269/G269</f>
+        <v>5.748199519871966E-2</v>
       </c>
       <c r="I269" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J269" s="16"/>
       <c r="K269" t="s">
@@ -11700,54 +11739,66 @@
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" s="9" t="s">
-        <v>511</v>
+        <v>135</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>517</v>
+        <v>520</v>
+      </c>
+      <c r="C270" s="18">
+        <v>161.97</v>
+      </c>
+      <c r="D270" s="17">
+        <v>3643312</v>
       </c>
       <c r="E270" s="10">
-        <v>788</v>
-      </c>
-      <c r="F270" s="14">
-        <v>62951</v>
+        <v>1293</v>
+      </c>
+      <c r="F270">
+        <v>137560</v>
       </c>
       <c r="G270" s="11">
-        <v>14271</v>
+        <v>22494</v>
       </c>
       <c r="H270" s="12">
         <f t="shared" si="12"/>
-        <v>5.521687337958097E-2</v>
+        <v>5.748199519871966E-2</v>
       </c>
       <c r="I270" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J270" s="16"/>
       <c r="K270" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="B271" s="15" t="s">
-        <v>272</v>
+        <v>510</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="C271" s="18">
+        <v>97.14</v>
+      </c>
+      <c r="D271" s="17">
+        <v>1817481</v>
       </c>
       <c r="E271" s="10">
-        <v>159</v>
+        <v>708</v>
       </c>
       <c r="F271" s="14">
-        <v>14721</v>
+        <v>84933</v>
       </c>
       <c r="G271" s="11">
-        <v>3442</v>
+        <v>18709</v>
       </c>
       <c r="H271" s="12">
         <f t="shared" si="12"/>
-        <v>4.6194073213248109E-2</v>
+        <v>3.7842749478860439E-2</v>
       </c>
       <c r="I271" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J271" s="16"/>
       <c r="K271" t="s">
@@ -11756,43 +11807,117 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
+      </c>
+      <c r="C272" s="18">
+        <v>136.31</v>
+      </c>
+      <c r="D272" s="17">
+        <v>1945274</v>
       </c>
       <c r="E272" s="10">
-        <v>369</v>
+        <v>788</v>
       </c>
       <c r="F272" s="14">
-        <v>24765</v>
+        <v>62951</v>
       </c>
       <c r="G272" s="11">
-        <v>6459</v>
+        <v>14271</v>
       </c>
       <c r="H272" s="12">
         <f t="shared" si="12"/>
-        <v>5.7129586623316304E-2</v>
+        <v>5.521687337958097E-2</v>
       </c>
       <c r="I272" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J272" s="16"/>
       <c r="K272" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B273" s="13"/>
-    </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B274" s="13"/>
-    </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A273" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B273" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C273" s="18">
+        <v>99.63</v>
+      </c>
+      <c r="D273" s="17">
+        <v>342925</v>
+      </c>
+      <c r="E273" s="10">
+        <v>159</v>
+      </c>
+      <c r="F273" s="14">
+        <v>14721</v>
+      </c>
+      <c r="G273" s="11">
+        <v>3442</v>
+      </c>
+      <c r="H273" s="12">
+        <f t="shared" si="12"/>
+        <v>4.6194073213248109E-2</v>
+      </c>
+      <c r="I273" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="J273" s="16"/>
+      <c r="K273" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A274" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="B274" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="C274">
+        <v>119.96</v>
+      </c>
+      <c r="D274" s="17">
+        <v>1817481</v>
+      </c>
+      <c r="E274" s="10">
+        <v>369</v>
+      </c>
+      <c r="F274" s="14">
+        <v>24765</v>
+      </c>
+      <c r="G274" s="11">
+        <v>6459</v>
+      </c>
+      <c r="H274" s="12">
+        <f t="shared" si="12"/>
+        <v>5.7129586623316304E-2</v>
+      </c>
+      <c r="I274" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="J274" s="16"/>
+      <c r="K274" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B275" s="13"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B276" s="13"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B277" s="13"/>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B278" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>